<commit_message>
bgdpbes, csc, bfpat, webapp
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\PA\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A1BF624-FC1F-45A1-A47D-F1FB76E9DD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E78EFCD1-C228-4458-BBD4-21755B5FE344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1970" yWindow="2020" windowWidth="14400" windowHeight="7350" firstSheet="2" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="285" yWindow="1515" windowWidth="16035" windowHeight="14175" firstSheet="2" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,9 +511,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -521,20 +521,20 @@
         <v>35</v>
       </c>
       <c r="C1" s="2">
-        <v>45330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+        <v>45362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -563,12 +563,12 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -615,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -678,17 +678,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -708,16 +708,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AE7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:AE25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -812,1337 +812,1337 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE2">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD3">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE3">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD4">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE4">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD5">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE5">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE8">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD10">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE10">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD13">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE13">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD14">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE14">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE15">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2332,764 +2332,764 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE18">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE19">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD20">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE20">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD21">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE21">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD22">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE22">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD23">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE23">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD24">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE24">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="L25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="M25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="N25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="O25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Q25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="R25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="S25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="T25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="U25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="V25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="W25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="X25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Y25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="Z25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AA25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AB25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AC25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AD25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AE25">
-        <v>0.33</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>